<commit_message>
gantt and scrum updated
</commit_message>
<xml_diff>
--- a/Boomberman/doku/210_Gantt-Diagramm_Joey_Alen.110.xlsx
+++ b/Boomberman/doku/210_Gantt-Diagramm_Joey_Alen.110.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Balkenplan" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="38">
   <si>
     <t>Nr.</t>
   </si>
@@ -32,24 +32,8 @@
     <t xml:space="preserve">Meilensteine </t>
   </si>
   <si>
-    <t>[Vorname 1] SOLL</t>
-  </si>
-  <si>
     <t>Dauer
 [geplant / wirklich]</t>
-  </si>
-  <si>
-    <t>[Vorname 1] IST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Vorname 1] IST
-</t>
-  </si>
-  <si>
-    <t>[Vorname 2] SOLL</t>
-  </si>
-  <si>
-    <t>[Vorname 2] IST</t>
   </si>
   <si>
     <t>geplant (SOLL)</t>
@@ -58,56 +42,102 @@
     <t>wirklich (IST)</t>
   </si>
   <si>
-    <t>4h / 2h</t>
-  </si>
-  <si>
-    <t>US 01 "Benutzer meldet sich an" implementieren</t>
-  </si>
-  <si>
     <t>Tätigkeiten / User Stories</t>
   </si>
   <si>
-    <t>US 02 "Benutzer meldet sich an" implementieren</t>
+    <t>Als Spieler möchte ich mir vor dem Spiel einen Namen geben.</t>
   </si>
   <si>
-    <t>US 03 "Benutzer meldet sich an" implementieren</t>
+    <t xml:space="preserve">Als Spieler möchte ich erst das Spiel starten können, wenn mein Gegner auch bereit ist (Namen eingegeben hat und auf Spiel starten gedrückt hat). </t>
   </si>
   <si>
-    <t>US 04 "Benutzer meldet sich an" implementieren</t>
+    <t>Als Spieler möchte ich am Anfang des Spiels die Map mit dem Spieltimer sehen können.</t>
   </si>
   <si>
-    <t>US 05 "Benutzer meldet sich an" implementieren</t>
+    <t>Als Spieler möchte ich mich mit entsprechenden Tasten bewegen können.</t>
   </si>
   <si>
-    <t>US 06 "Benutzer meldet sich an" implementieren</t>
+    <t>Als Spieler möchte ich eine Bombe legen können, die nach einem Timer von 3 Sekunden explodiert.</t>
   </si>
   <si>
-    <t>US 07 "Benutzer meldet sich an" implementieren</t>
+    <t>Als Spieler möchte ich den anderen Spieler sehen können, da das Spiel über das Netzwerk (Socket) läuft.</t>
   </si>
   <si>
-    <t>US 08 "Benutzer meldet sich an" implementieren</t>
+    <t>Als Spieler möchte ich sehen wieviele Lebenspunkte mir abgezogen worden sind durch die explodierte Bombe.</t>
   </si>
   <si>
-    <t>US 09 "Benutzer meldet sich an" implementieren</t>
+    <t>Als Spieler möchte ich sehen können wie viele Lebenspunkte ich und mein Gegner noch haben.</t>
   </si>
   <si>
-    <t>US 10 "Benutzer meldet sich an" implementieren</t>
+    <t xml:space="preserve">Als Spieler möchte ich nach einem Spiel auswählen können, ob ich erneut spielen möchte oder das Programm beenden möchte. </t>
   </si>
   <si>
-    <t>US 11 "Benutzer meldet sich an" implementieren</t>
+    <t>Als Spieler möchte ich sehen, wer verloren hat und wer gewonnen hat.</t>
   </si>
   <si>
-    <t>US 12 "Benutzer meldet sich an" implementieren</t>
+    <t>Als Spieler möchte ich, dass der Timer zu Spielbeginn von 5min herunterzählt.</t>
   </si>
   <si>
-    <t>US 13 "Benutzer meldet sich an" implementieren</t>
+    <t>Als Spieler möchte ich zwischen 3 verschiedenen Maps auswählen können.</t>
+  </si>
+  <si>
+    <t>Als Spieler möchte ich mir die Highscores ansehen können, indem ich auf den Highscorebutton drücke.</t>
+  </si>
+  <si>
+    <t>Als Projektleiter möchte ich, dass die Dokumentation(Teil1) am Mittwoch 12:00 Uhr komplett fertig ist.</t>
+  </si>
+  <si>
+    <t>Als Projektleiter möchte ich, dass der Sourcecode übersichtlich und strukturiert gehalten / geschrieben wird, um Komplikationen zu vermeiden.</t>
+  </si>
+  <si>
+    <t>3h / 2h</t>
+  </si>
+  <si>
+    <t>Nico SOLL</t>
+  </si>
+  <si>
+    <t>Nico IST</t>
+  </si>
+  <si>
+    <t>Joey SOLL</t>
+  </si>
+  <si>
+    <t>3h / 3h</t>
+  </si>
+  <si>
+    <t>6h /</t>
+  </si>
+  <si>
+    <t>8h /</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4h / </t>
+  </si>
+  <si>
+    <t>5h /</t>
+  </si>
+  <si>
+    <t>3h /</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3h / </t>
+  </si>
+  <si>
+    <t>2h / 1h</t>
+  </si>
+  <si>
+    <t>Joey IST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nico IST
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +202,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -216,7 +253,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -352,13 +389,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1"/>
@@ -433,15 +510,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -451,8 +519,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -460,19 +528,16 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -482,7 +547,22 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -499,21 +579,32 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="60 % - Akzent1" xfId="2" builtinId="32"/>
@@ -826,10 +917,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CG68"/>
+  <dimension ref="A1:CG64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,7 +963,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:85" s="2" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="24"/>
@@ -881,120 +972,120 @@
         <v>2</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="61">
+        <v>31.01</v>
+      </c>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="61">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="61">
+        <v>6.02</v>
+      </c>
+      <c r="W1" s="62"/>
+      <c r="X1" s="62"/>
+      <c r="Y1" s="62"/>
+      <c r="Z1" s="62"/>
+      <c r="AA1" s="62"/>
+      <c r="AB1" s="62"/>
+      <c r="AC1" s="63"/>
+      <c r="AD1" s="61">
+        <v>7.02</v>
+      </c>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="62"/>
+      <c r="AG1" s="62"/>
+      <c r="AH1" s="62"/>
+      <c r="AI1" s="62"/>
+      <c r="AJ1" s="62"/>
+      <c r="AK1" s="63"/>
+      <c r="AL1" s="61">
+        <v>19.02</v>
+      </c>
+      <c r="AM1" s="62"/>
+      <c r="AN1" s="62"/>
+      <c r="AO1" s="62"/>
+      <c r="AP1" s="62"/>
+      <c r="AQ1" s="62"/>
+      <c r="AR1" s="62"/>
+      <c r="AS1" s="63"/>
+      <c r="AT1" s="61">
+        <v>20.02</v>
+      </c>
+      <c r="AU1" s="62"/>
+      <c r="AV1" s="62"/>
+      <c r="AW1" s="62"/>
+      <c r="AX1" s="62"/>
+      <c r="AY1" s="62"/>
+      <c r="AZ1" s="62"/>
+      <c r="BA1" s="63"/>
+      <c r="BB1" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="46" t="s">
+      <c r="BC1" s="62"/>
+      <c r="BD1" s="62"/>
+      <c r="BE1" s="62"/>
+      <c r="BF1" s="62"/>
+      <c r="BG1" s="62"/>
+      <c r="BH1" s="62"/>
+      <c r="BI1" s="63"/>
+      <c r="BJ1" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="48"/>
-      <c r="V1" s="46" t="s">
+      <c r="BK1" s="62"/>
+      <c r="BL1" s="62"/>
+      <c r="BM1" s="62"/>
+      <c r="BN1" s="62"/>
+      <c r="BO1" s="62"/>
+      <c r="BP1" s="62"/>
+      <c r="BQ1" s="63"/>
+      <c r="BR1" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="48"/>
-      <c r="AD1" s="46" t="s">
+      <c r="BS1" s="62"/>
+      <c r="BT1" s="62"/>
+      <c r="BU1" s="62"/>
+      <c r="BV1" s="62"/>
+      <c r="BW1" s="62"/>
+      <c r="BX1" s="62"/>
+      <c r="BY1" s="63"/>
+      <c r="BZ1" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="AE1" s="47"/>
-      <c r="AF1" s="47"/>
-      <c r="AG1" s="47"/>
-      <c r="AH1" s="47"/>
-      <c r="AI1" s="47"/>
-      <c r="AJ1" s="47"/>
-      <c r="AK1" s="48"/>
-      <c r="AL1" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="AM1" s="47"/>
-      <c r="AN1" s="47"/>
-      <c r="AO1" s="47"/>
-      <c r="AP1" s="47"/>
-      <c r="AQ1" s="47"/>
-      <c r="AR1" s="47"/>
-      <c r="AS1" s="48"/>
-      <c r="AT1" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="AU1" s="47"/>
-      <c r="AV1" s="47"/>
-      <c r="AW1" s="47"/>
-      <c r="AX1" s="47"/>
-      <c r="AY1" s="47"/>
-      <c r="AZ1" s="47"/>
-      <c r="BA1" s="48"/>
-      <c r="BB1" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="BC1" s="47"/>
-      <c r="BD1" s="47"/>
-      <c r="BE1" s="47"/>
-      <c r="BF1" s="47"/>
-      <c r="BG1" s="47"/>
-      <c r="BH1" s="47"/>
-      <c r="BI1" s="48"/>
-      <c r="BJ1" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="BK1" s="47"/>
-      <c r="BL1" s="47"/>
-      <c r="BM1" s="47"/>
-      <c r="BN1" s="47"/>
-      <c r="BO1" s="47"/>
-      <c r="BP1" s="47"/>
-      <c r="BQ1" s="48"/>
-      <c r="BR1" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="BS1" s="47"/>
-      <c r="BT1" s="47"/>
-      <c r="BU1" s="47"/>
-      <c r="BV1" s="47"/>
-      <c r="BW1" s="47"/>
-      <c r="BX1" s="47"/>
-      <c r="BY1" s="48"/>
-      <c r="BZ1" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="CA1" s="47"/>
-      <c r="CB1" s="47"/>
-      <c r="CC1" s="47"/>
-      <c r="CD1" s="47"/>
-      <c r="CE1" s="47"/>
-      <c r="CF1" s="47"/>
-      <c r="CG1" s="48"/>
+      <c r="CA1" s="62"/>
+      <c r="CB1" s="62"/>
+      <c r="CC1" s="62"/>
+      <c r="CD1" s="62"/>
+      <c r="CE1" s="62"/>
+      <c r="CF1" s="62"/>
+      <c r="CG1" s="63"/>
     </row>
     <row r="2" spans="1:85" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="62"/>
+      <c r="A2" s="60"/>
       <c r="B2" s="22" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="29"/>
       <c r="E2" s="45" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F2" s="3">
         <v>1</v>
@@ -1238,21 +1329,22 @@
       </c>
     </row>
     <row r="3" spans="1:85" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52">
+      <c r="A3" s="58">
         <v>1</v>
       </c>
-      <c r="B3" s="49" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="63" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="63"/>
-      <c r="E3" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="66"/>
-      <c r="G3" s="67"/>
+      <c r="B3" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="64" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="64"/>
+      <c r="E3" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="42"/>
       <c r="M3" s="11"/>
       <c r="N3" s="9"/>
       <c r="U3" s="11"/>
@@ -1273,15 +1365,16 @@
       <c r="BZ3" s="9"/>
       <c r="CG3" s="11"/>
     </row>
-    <row r="4" spans="1:85" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="23"/>
+    <row r="4" spans="1:85" s="12" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="58"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
       <c r="M4" s="13"/>
       <c r="U4" s="13"/>
       <c r="AC4" s="13"/>
@@ -1294,15 +1387,13 @@
       <c r="CG4" s="13"/>
     </row>
     <row r="5" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="27" t="s">
+        <v>27</v>
+      </c>
       <c r="M5" s="13"/>
       <c r="U5" s="13"/>
       <c r="AC5" s="13"/>
@@ -1314,16 +1405,16 @@
       <c r="BY5" s="13"/>
       <c r="CG5" s="13"/>
     </row>
-    <row r="6" spans="1:85" s="14" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A6" s="52"/>
-      <c r="B6" s="61"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="40" t="s">
-        <v>10</v>
+    <row r="6" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="58"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="43" t="s">
+        <v>36</v>
       </c>
       <c r="F6" s="12"/>
-      <c r="G6" s="23"/>
+      <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -1404,16 +1495,18 @@
       <c r="CG6" s="13"/>
     </row>
     <row r="7" spans="1:85" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="52">
+      <c r="A7" s="58">
         <v>2</v>
       </c>
-      <c r="B7" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="55"/>
-      <c r="D7" s="56"/>
+      <c r="B7" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="69" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="70"/>
       <c r="E7" s="26" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F7" s="15"/>
       <c r="M7" s="17"/>
@@ -1423,8 +1516,14 @@
       <c r="AC7" s="17"/>
       <c r="AD7" s="15"/>
       <c r="AK7" s="17"/>
-      <c r="AL7" s="15"/>
-      <c r="AS7" s="17"/>
+      <c r="AL7" s="75"/>
+      <c r="AM7" s="73"/>
+      <c r="AN7" s="73"/>
+      <c r="AO7" s="73"/>
+      <c r="AP7" s="73"/>
+      <c r="AQ7" s="73"/>
+      <c r="AR7" s="73"/>
+      <c r="AS7" s="76"/>
       <c r="AT7" s="15"/>
       <c r="BA7" s="17"/>
       <c r="BB7" s="15"/>
@@ -1437,12 +1536,12 @@
       <c r="CG7" s="17"/>
     </row>
     <row r="8" spans="1:85" s="19" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
-      <c r="B8" s="60"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="58"/>
+      <c r="A8" s="58"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="72"/>
       <c r="E8" s="43" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="F8" s="18"/>
       <c r="M8" s="20"/>
@@ -1466,12 +1565,12 @@
       <c r="CG8" s="20"/>
     </row>
     <row r="9" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
-      <c r="B9" s="60"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="58"/>
+      <c r="A9" s="58"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="72"/>
       <c r="E9" s="27" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="F9" s="18"/>
       <c r="M9" s="20"/>
@@ -1481,8 +1580,14 @@
       <c r="AC9" s="20"/>
       <c r="AD9" s="18"/>
       <c r="AK9" s="20"/>
-      <c r="AL9" s="18"/>
-      <c r="AS9" s="20"/>
+      <c r="AL9" s="81"/>
+      <c r="AM9" s="42"/>
+      <c r="AN9" s="42"/>
+      <c r="AO9" s="42"/>
+      <c r="AP9" s="42"/>
+      <c r="AQ9" s="42"/>
+      <c r="AR9" s="42"/>
+      <c r="AS9" s="79"/>
       <c r="AT9" s="18"/>
       <c r="BA9" s="20"/>
       <c r="BB9" s="18"/>
@@ -1494,13 +1599,13 @@
       <c r="BZ9" s="18"/>
       <c r="CG9" s="20"/>
     </row>
-    <row r="10" spans="1:85" s="21" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="52"/>
-      <c r="B10" s="61"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
+    <row r="10" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="58"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72"/>
       <c r="E10" s="43" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F10" s="18"/>
       <c r="G10" s="19"/>
@@ -1584,22 +1689,27 @@
       <c r="CG10" s="20"/>
     </row>
     <row r="11" spans="1:85" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="52">
+      <c r="A11" s="58">
         <v>3</v>
       </c>
-      <c r="B11" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
+      <c r="B11" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="64"/>
       <c r="E11" s="39" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F11" s="9"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="9"/>
+      <c r="N11" s="82"/>
       <c r="U11" s="11"/>
       <c r="V11" s="9"/>
+      <c r="W11" s="73"/>
+      <c r="X11" s="73"/>
+      <c r="Y11" s="73"/>
+      <c r="Z11" s="73"/>
       <c r="AC11" s="11"/>
       <c r="AD11" s="9"/>
       <c r="AK11" s="11"/>
@@ -1616,15 +1726,15 @@
       <c r="BZ11" s="9"/>
       <c r="CG11" s="11"/>
     </row>
-    <row r="12" spans="1:85" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A12" s="52"/>
-      <c r="B12" s="60"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
+    <row r="12" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="58"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="65"/>
       <c r="E12" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="M12" s="13"/>
+        <v>26</v>
+      </c>
+      <c r="N12" s="83"/>
       <c r="U12" s="13"/>
       <c r="AC12" s="13"/>
       <c r="AK12" s="13"/>
@@ -1636,15 +1746,19 @@
       <c r="CG12" s="13"/>
     </row>
     <row r="13" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="52"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
+      <c r="A13" s="58"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
       <c r="E13" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="M13" s="13"/>
+        <v>27</v>
+      </c>
+      <c r="M13" s="84"/>
       <c r="U13" s="13"/>
+      <c r="W13" s="42"/>
+      <c r="X13" s="42"/>
+      <c r="Y13" s="42"/>
+      <c r="Z13" s="42"/>
       <c r="AC13" s="13"/>
       <c r="AK13" s="13"/>
       <c r="AS13" s="13"/>
@@ -1654,13 +1768,13 @@
       <c r="BY13" s="13"/>
       <c r="CG13" s="13"/>
     </row>
-    <row r="14" spans="1:85" s="14" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A14" s="52"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
+    <row r="14" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="58"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
       <c r="E14" s="40" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -1669,8 +1783,8 @@
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="80"/>
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="12"/>
@@ -1744,18 +1858,19 @@
       <c r="CG14" s="13"/>
     </row>
     <row r="15" spans="1:85" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="52">
+      <c r="A15" s="58">
         <v>4</v>
       </c>
-      <c r="B15" s="49" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="55"/>
-      <c r="D15" s="56"/>
+      <c r="B15" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="69" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="70"/>
       <c r="E15" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="15"/>
+        <v>25</v>
+      </c>
       <c r="M15" s="17"/>
       <c r="N15" s="15"/>
       <c r="U15" s="17"/>
@@ -1776,15 +1891,14 @@
       <c r="BZ15" s="15"/>
       <c r="CG15" s="17"/>
     </row>
-    <row r="16" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="52"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="18"/>
+    <row r="16" spans="1:85" s="19" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="58"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="43" t="s">
+        <v>37</v>
+      </c>
       <c r="M16" s="20"/>
       <c r="N16" s="18"/>
       <c r="U16" s="20"/>
@@ -1806,14 +1920,17 @@
       <c r="CG16" s="20"/>
     </row>
     <row r="17" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="52"/>
-      <c r="B17" s="60"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="58"/>
+      <c r="A17" s="58"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="72"/>
       <c r="E17" s="27" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="F17" s="18"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="73"/>
       <c r="M17" s="20"/>
       <c r="N17" s="18"/>
       <c r="U17" s="20"/>
@@ -1834,19 +1951,19 @@
       <c r="BZ17" s="18"/>
       <c r="CG17" s="20"/>
     </row>
-    <row r="18" spans="1:85" s="21" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="52"/>
-      <c r="B18" s="61"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58"/>
+    <row r="18" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="58"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="72"/>
       <c r="E18" s="43" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
+      <c r="H18" s="74"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
       <c r="K18" s="19"/>
       <c r="L18" s="19"/>
       <c r="M18" s="20"/>
@@ -1924,20 +2041,21 @@
       <c r="CG18" s="20"/>
     </row>
     <row r="19" spans="1:85" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="52">
+      <c r="A19" s="58">
         <v>5</v>
       </c>
-      <c r="B19" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="39" t="s">
-        <v>5</v>
+      <c r="B19" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="64" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="64"/>
+      <c r="E19" s="26" t="s">
+        <v>25</v>
       </c>
       <c r="F19" s="9"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="9"/>
+      <c r="N19" s="82"/>
       <c r="U19" s="11"/>
       <c r="V19" s="9"/>
       <c r="AC19" s="11"/>
@@ -1956,15 +2074,15 @@
       <c r="BZ19" s="9"/>
       <c r="CG19" s="11"/>
     </row>
-    <row r="20" spans="1:85" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A20" s="52"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="M20" s="13"/>
+    <row r="20" spans="1:85" s="12" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="58"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="N20" s="80"/>
       <c r="U20" s="13"/>
       <c r="AC20" s="13"/>
       <c r="AK20" s="13"/>
@@ -1976,14 +2094,19 @@
       <c r="CG20" s="13"/>
     </row>
     <row r="21" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="52"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="M21" s="13"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="K21" s="73"/>
+      <c r="L21" s="73"/>
+      <c r="M21" s="76"/>
+      <c r="N21" s="75"/>
+      <c r="O21" s="73"/>
+      <c r="P21" s="73"/>
       <c r="U21" s="13"/>
       <c r="AC21" s="13"/>
       <c r="AK21" s="13"/>
@@ -1994,22 +2117,22 @@
       <c r="BY21" s="13"/>
       <c r="CG21" s="13"/>
     </row>
-    <row r="22" spans="1:85" s="14" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A22" s="52"/>
-      <c r="B22" s="61"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="40" t="s">
-        <v>10</v>
+    <row r="22" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="58"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="43" t="s">
+        <v>36</v>
       </c>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="13"/>
+      <c r="K22" s="77"/>
+      <c r="L22" s="77"/>
+      <c r="M22" s="78"/>
       <c r="N22" s="12"/>
       <c r="O22" s="12"/>
       <c r="P22" s="12"/>
@@ -2084,22 +2207,28 @@
       <c r="CG22" s="13"/>
     </row>
     <row r="23" spans="1:85" s="16" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="52">
+      <c r="A23" s="58">
         <v>6</v>
       </c>
-      <c r="B23" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="55"/>
-      <c r="D23" s="56"/>
+      <c r="B23" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="70"/>
       <c r="E23" s="26" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F23" s="15"/>
       <c r="M23" s="17"/>
       <c r="N23" s="15"/>
-      <c r="U23" s="17"/>
-      <c r="V23" s="15"/>
+      <c r="Q23" s="73"/>
+      <c r="R23" s="73"/>
+      <c r="S23" s="73"/>
+      <c r="T23" s="73"/>
+      <c r="U23" s="76"/>
+      <c r="V23" s="75"/>
       <c r="AC23" s="17"/>
       <c r="AD23" s="15"/>
       <c r="AK23" s="17"/>
@@ -2116,13 +2245,13 @@
       <c r="BZ23" s="15"/>
       <c r="CG23" s="17"/>
     </row>
-    <row r="24" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="52"/>
-      <c r="B24" s="60"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="27" t="s">
-        <v>8</v>
+    <row r="24" spans="1:85" s="19" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="58"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="43" t="s">
+        <v>37</v>
       </c>
       <c r="F24" s="18"/>
       <c r="M24" s="20"/>
@@ -2146,18 +2275,22 @@
       <c r="CG24" s="20"/>
     </row>
     <row r="25" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="52"/>
-      <c r="B25" s="60"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="58"/>
+      <c r="A25" s="58"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="72"/>
       <c r="E25" s="27" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="F25" s="18"/>
       <c r="M25" s="20"/>
       <c r="N25" s="18"/>
-      <c r="U25" s="20"/>
-      <c r="V25" s="18"/>
+      <c r="Q25" s="42"/>
+      <c r="R25" s="42"/>
+      <c r="S25" s="42"/>
+      <c r="T25" s="42"/>
+      <c r="U25" s="79"/>
+      <c r="V25" s="81"/>
       <c r="AC25" s="20"/>
       <c r="AD25" s="18"/>
       <c r="AK25" s="20"/>
@@ -2174,13 +2307,13 @@
       <c r="BZ25" s="18"/>
       <c r="CG25" s="20"/>
     </row>
-    <row r="26" spans="1:85" s="21" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="52"/>
-      <c r="B26" s="61"/>
-      <c r="C26" s="58"/>
-      <c r="D26" s="58"/>
+    <row r="26" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="58"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="72"/>
+      <c r="D26" s="72"/>
       <c r="E26" s="43" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F26" s="18"/>
       <c r="G26" s="19"/>
@@ -2264,24 +2397,29 @@
       <c r="CG26" s="20"/>
     </row>
     <row r="27" spans="1:85" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="52">
+      <c r="A27" s="58">
         <v>7</v>
       </c>
-      <c r="B27" s="49" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="49"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="39" t="s">
-        <v>5</v>
+      <c r="B27" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="64" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="64"/>
+      <c r="E27" s="26" t="s">
+        <v>25</v>
       </c>
       <c r="F27" s="9"/>
       <c r="M27" s="11"/>
       <c r="N27" s="9"/>
       <c r="U27" s="11"/>
       <c r="V27" s="9"/>
-      <c r="AC27" s="11"/>
-      <c r="AD27" s="9"/>
+      <c r="AA27" s="73"/>
+      <c r="AB27" s="73"/>
+      <c r="AC27" s="76"/>
+      <c r="AD27" s="75"/>
+      <c r="AE27" s="73"/>
       <c r="AK27" s="11"/>
       <c r="AL27" s="9"/>
       <c r="AS27" s="11"/>
@@ -2296,13 +2434,13 @@
       <c r="BZ27" s="9"/>
       <c r="CG27" s="11"/>
     </row>
-    <row r="28" spans="1:85" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A28" s="52"/>
-      <c r="B28" s="60"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="40" t="s">
-        <v>7</v>
+    <row r="28" spans="1:85" s="12" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="58"/>
+      <c r="B28" s="56"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="43" t="s">
+        <v>37</v>
       </c>
       <c r="M28" s="13"/>
       <c r="U28" s="13"/>
@@ -2316,16 +2454,20 @@
       <c r="CG28" s="13"/>
     </row>
     <row r="29" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="52"/>
-      <c r="B29" s="60"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="41" t="s">
-        <v>9</v>
+      <c r="A29" s="58"/>
+      <c r="B29" s="56"/>
+      <c r="C29" s="65"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="27" t="s">
+        <v>27</v>
       </c>
       <c r="M29" s="13"/>
       <c r="U29" s="13"/>
-      <c r="AC29" s="13"/>
+      <c r="AA29" s="42"/>
+      <c r="AB29" s="42"/>
+      <c r="AC29" s="79"/>
+      <c r="AD29" s="42"/>
+      <c r="AE29" s="42"/>
       <c r="AK29" s="13"/>
       <c r="AS29" s="13"/>
       <c r="BA29" s="13"/>
@@ -2334,13 +2476,13 @@
       <c r="BY29" s="13"/>
       <c r="CG29" s="13"/>
     </row>
-    <row r="30" spans="1:85" s="14" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A30" s="52"/>
-      <c r="B30" s="61"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="40" t="s">
-        <v>10</v>
+    <row r="30" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="58"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="43" t="s">
+        <v>36</v>
       </c>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
@@ -2424,16 +2566,18 @@
       <c r="CG30" s="13"/>
     </row>
     <row r="31" spans="1:85" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="52">
+      <c r="A31" s="58">
         <v>8</v>
       </c>
-      <c r="B31" s="49" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="55"/>
-      <c r="D31" s="56"/>
+      <c r="B31" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="70"/>
       <c r="E31" s="26" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F31" s="15"/>
       <c r="M31" s="17"/>
@@ -2442,6 +2586,9 @@
       <c r="V31" s="15"/>
       <c r="AC31" s="17"/>
       <c r="AD31" s="15"/>
+      <c r="AF31" s="73"/>
+      <c r="AG31" s="73"/>
+      <c r="AH31" s="73"/>
       <c r="AK31" s="17"/>
       <c r="AL31" s="15"/>
       <c r="AS31" s="17"/>
@@ -2456,13 +2603,13 @@
       <c r="BZ31" s="15"/>
       <c r="CG31" s="17"/>
     </row>
-    <row r="32" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="52"/>
-      <c r="B32" s="60"/>
-      <c r="C32" s="57"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="27" t="s">
-        <v>8</v>
+    <row r="32" spans="1:85" s="19" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="58"/>
+      <c r="B32" s="56"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="72"/>
+      <c r="E32" s="43" t="s">
+        <v>37</v>
       </c>
       <c r="F32" s="18"/>
       <c r="M32" s="20"/>
@@ -2486,12 +2633,12 @@
       <c r="CG32" s="20"/>
     </row>
     <row r="33" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="52"/>
-      <c r="B33" s="60"/>
-      <c r="C33" s="57"/>
-      <c r="D33" s="58"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="56"/>
+      <c r="C33" s="71"/>
+      <c r="D33" s="72"/>
       <c r="E33" s="27" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="F33" s="18"/>
       <c r="M33" s="20"/>
@@ -2500,6 +2647,9 @@
       <c r="V33" s="18"/>
       <c r="AC33" s="20"/>
       <c r="AD33" s="18"/>
+      <c r="AF33" s="42"/>
+      <c r="AG33" s="42"/>
+      <c r="AH33" s="42"/>
       <c r="AK33" s="20"/>
       <c r="AL33" s="18"/>
       <c r="AS33" s="20"/>
@@ -2514,13 +2664,13 @@
       <c r="BZ33" s="18"/>
       <c r="CG33" s="20"/>
     </row>
-    <row r="34" spans="1:85" s="21" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="52"/>
-      <c r="B34" s="61"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="58"/>
+    <row r="34" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="58"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="72"/>
+      <c r="D34" s="72"/>
       <c r="E34" s="43" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F34" s="18"/>
       <c r="G34" s="19"/>
@@ -2604,16 +2754,18 @@
       <c r="CG34" s="20"/>
     </row>
     <row r="35" spans="1:85" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="52">
+      <c r="A35" s="58">
         <v>9</v>
       </c>
-      <c r="B35" s="49" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="39" t="s">
-        <v>5</v>
+      <c r="B35" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="64"/>
+      <c r="E35" s="26" t="s">
+        <v>25</v>
       </c>
       <c r="F35" s="9"/>
       <c r="M35" s="11"/>
@@ -2626,6 +2778,10 @@
       <c r="AL35" s="9"/>
       <c r="AS35" s="11"/>
       <c r="AT35" s="9"/>
+      <c r="AW35" s="73"/>
+      <c r="AX35" s="73"/>
+      <c r="AY35" s="73"/>
+      <c r="AZ35" s="73"/>
       <c r="BA35" s="11"/>
       <c r="BB35" s="9"/>
       <c r="BI35" s="11"/>
@@ -2636,13 +2792,13 @@
       <c r="BZ35" s="9"/>
       <c r="CG35" s="11"/>
     </row>
-    <row r="36" spans="1:85" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A36" s="52"/>
-      <c r="B36" s="60"/>
-      <c r="C36" s="50"/>
-      <c r="D36" s="50"/>
-      <c r="E36" s="40" t="s">
-        <v>7</v>
+    <row r="36" spans="1:85" s="12" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="58"/>
+      <c r="B36" s="56"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="65"/>
+      <c r="E36" s="43" t="s">
+        <v>37</v>
       </c>
       <c r="M36" s="13"/>
       <c r="U36" s="13"/>
@@ -2656,31 +2812,35 @@
       <c r="CG36" s="13"/>
     </row>
     <row r="37" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="52"/>
-      <c r="B37" s="60"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="50"/>
-      <c r="E37" s="41" t="s">
-        <v>9</v>
+      <c r="A37" s="58"/>
+      <c r="B37" s="56"/>
+      <c r="C37" s="65"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="27" t="s">
+        <v>27</v>
       </c>
       <c r="M37" s="13"/>
       <c r="U37" s="13"/>
       <c r="AC37" s="13"/>
       <c r="AK37" s="13"/>
       <c r="AS37" s="13"/>
+      <c r="AW37" s="42"/>
+      <c r="AX37" s="42"/>
+      <c r="AY37" s="42"/>
+      <c r="AZ37" s="42"/>
       <c r="BA37" s="13"/>
       <c r="BI37" s="13"/>
       <c r="BQ37" s="13"/>
       <c r="BY37" s="13"/>
       <c r="CG37" s="13"/>
     </row>
-    <row r="38" spans="1:85" s="14" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A38" s="52"/>
-      <c r="B38" s="61"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="51"/>
-      <c r="E38" s="40" t="s">
-        <v>10</v>
+    <row r="38" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="58"/>
+      <c r="B38" s="57"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="43" t="s">
+        <v>36</v>
       </c>
       <c r="F38" s="12"/>
       <c r="G38" s="12"/>
@@ -2764,16 +2924,18 @@
       <c r="CG38" s="13"/>
     </row>
     <row r="39" spans="1:85" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="52">
+      <c r="A39" s="58">
         <v>10</v>
       </c>
-      <c r="B39" s="49" t="s">
-        <v>24</v>
-      </c>
-      <c r="C39" s="55"/>
-      <c r="D39" s="56"/>
+      <c r="B39" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="70"/>
       <c r="E39" s="26" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F39" s="15"/>
       <c r="M39" s="17"/>
@@ -2785,7 +2947,9 @@
       <c r="AK39" s="17"/>
       <c r="AL39" s="15"/>
       <c r="AS39" s="17"/>
-      <c r="AT39" s="15"/>
+      <c r="AT39" s="75"/>
+      <c r="AU39" s="73"/>
+      <c r="AV39" s="73"/>
       <c r="BA39" s="17"/>
       <c r="BB39" s="15"/>
       <c r="BI39" s="17"/>
@@ -2796,13 +2960,13 @@
       <c r="BZ39" s="15"/>
       <c r="CG39" s="17"/>
     </row>
-    <row r="40" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="52"/>
-      <c r="B40" s="60"/>
-      <c r="C40" s="57"/>
-      <c r="D40" s="58"/>
-      <c r="E40" s="27" t="s">
-        <v>8</v>
+    <row r="40" spans="1:85" s="19" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="58"/>
+      <c r="B40" s="56"/>
+      <c r="C40" s="71"/>
+      <c r="D40" s="72"/>
+      <c r="E40" s="43" t="s">
+        <v>37</v>
       </c>
       <c r="F40" s="18"/>
       <c r="M40" s="20"/>
@@ -2826,12 +2990,12 @@
       <c r="CG40" s="20"/>
     </row>
     <row r="41" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="52"/>
-      <c r="B41" s="60"/>
-      <c r="C41" s="57"/>
-      <c r="D41" s="58"/>
+      <c r="A41" s="58"/>
+      <c r="B41" s="56"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="72"/>
       <c r="E41" s="27" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="F41" s="18"/>
       <c r="M41" s="20"/>
@@ -2843,7 +3007,9 @@
       <c r="AK41" s="20"/>
       <c r="AL41" s="18"/>
       <c r="AS41" s="20"/>
-      <c r="AT41" s="18"/>
+      <c r="AT41" s="81"/>
+      <c r="AU41" s="42"/>
+      <c r="AV41" s="42"/>
       <c r="BA41" s="20"/>
       <c r="BB41" s="18"/>
       <c r="BI41" s="20"/>
@@ -2854,13 +3020,13 @@
       <c r="BZ41" s="18"/>
       <c r="CG41" s="20"/>
     </row>
-    <row r="42" spans="1:85" s="21" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="52"/>
-      <c r="B42" s="61"/>
-      <c r="C42" s="58"/>
-      <c r="D42" s="58"/>
+    <row r="42" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="58"/>
+      <c r="B42" s="57"/>
+      <c r="C42" s="72"/>
+      <c r="D42" s="72"/>
       <c r="E42" s="43" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F42" s="18"/>
       <c r="G42" s="19"/>
@@ -2944,20 +3110,23 @@
       <c r="CG42" s="20"/>
     </row>
     <row r="43" spans="1:85" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="52">
+      <c r="A43" s="58">
         <v>11</v>
       </c>
-      <c r="B43" s="49" t="s">
+      <c r="B43" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="64" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" s="64"/>
+      <c r="E43" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C43" s="49"/>
-      <c r="D43" s="49"/>
-      <c r="E43" s="39" t="s">
-        <v>5</v>
-      </c>
       <c r="F43" s="9"/>
-      <c r="M43" s="11"/>
-      <c r="N43" s="9"/>
+      <c r="M43" s="73"/>
+      <c r="N43" s="85"/>
+      <c r="O43" s="73"/>
       <c r="U43" s="11"/>
       <c r="V43" s="9"/>
       <c r="AC43" s="11"/>
@@ -2976,15 +3145,15 @@
       <c r="BZ43" s="9"/>
       <c r="CG43" s="11"/>
     </row>
-    <row r="44" spans="1:85" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A44" s="52"/>
-      <c r="B44" s="60"/>
-      <c r="C44" s="50"/>
-      <c r="D44" s="50"/>
-      <c r="E44" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="M44" s="13"/>
+    <row r="44" spans="1:85" s="12" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="58"/>
+      <c r="B44" s="56"/>
+      <c r="C44" s="65"/>
+      <c r="D44" s="65"/>
+      <c r="E44" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="M44" s="86"/>
       <c r="U44" s="13"/>
       <c r="AC44" s="13"/>
       <c r="AK44" s="13"/>
@@ -2996,12 +3165,12 @@
       <c r="CG44" s="13"/>
     </row>
     <row r="45" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="52"/>
-      <c r="B45" s="60"/>
-      <c r="C45" s="50"/>
-      <c r="D45" s="50"/>
-      <c r="E45" s="41" t="s">
-        <v>9</v>
+      <c r="A45" s="58"/>
+      <c r="B45" s="56"/>
+      <c r="C45" s="65"/>
+      <c r="D45" s="65"/>
+      <c r="E45" s="27" t="s">
+        <v>27</v>
       </c>
       <c r="M45" s="13"/>
       <c r="U45" s="13"/>
@@ -3014,13 +3183,13 @@
       <c r="BY45" s="13"/>
       <c r="CG45" s="13"/>
     </row>
-    <row r="46" spans="1:85" s="14" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A46" s="52"/>
-      <c r="B46" s="61"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="51"/>
-      <c r="E46" s="40" t="s">
-        <v>10</v>
+    <row r="46" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="58"/>
+      <c r="B46" s="57"/>
+      <c r="C46" s="66"/>
+      <c r="D46" s="66"/>
+      <c r="E46" s="43" t="s">
+        <v>36</v>
       </c>
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
@@ -3104,16 +3273,18 @@
       <c r="CG46" s="13"/>
     </row>
     <row r="47" spans="1:85" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="52">
+      <c r="A47" s="58">
         <v>12</v>
       </c>
-      <c r="B47" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="C47" s="55"/>
-      <c r="D47" s="56"/>
+      <c r="B47" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="D47" s="70"/>
       <c r="E47" s="26" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F47" s="15"/>
       <c r="M47" s="17"/>
@@ -3136,13 +3307,13 @@
       <c r="BZ47" s="15"/>
       <c r="CG47" s="17"/>
     </row>
-    <row r="48" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="52"/>
-      <c r="B48" s="60"/>
-      <c r="C48" s="57"/>
-      <c r="D48" s="58"/>
-      <c r="E48" s="27" t="s">
-        <v>7</v>
+    <row r="48" spans="1:85" s="19" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="58"/>
+      <c r="B48" s="56"/>
+      <c r="C48" s="71"/>
+      <c r="D48" s="72"/>
+      <c r="E48" s="43" t="s">
+        <v>37</v>
       </c>
       <c r="F48" s="18"/>
       <c r="M48" s="20"/>
@@ -3166,12 +3337,12 @@
       <c r="CG48" s="20"/>
     </row>
     <row r="49" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="52"/>
-      <c r="B49" s="60"/>
-      <c r="C49" s="57"/>
-      <c r="D49" s="58"/>
+      <c r="A49" s="58"/>
+      <c r="B49" s="56"/>
+      <c r="C49" s="71"/>
+      <c r="D49" s="72"/>
       <c r="E49" s="27" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="F49" s="18"/>
       <c r="M49" s="20"/>
@@ -3194,13 +3365,13 @@
       <c r="BZ49" s="18"/>
       <c r="CG49" s="20"/>
     </row>
-    <row r="50" spans="1:85" s="21" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="52"/>
-      <c r="B50" s="61"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="58"/>
+    <row r="50" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="58"/>
+      <c r="B50" s="57"/>
+      <c r="C50" s="72"/>
+      <c r="D50" s="72"/>
       <c r="E50" s="43" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F50" s="18"/>
       <c r="G50" s="19"/>
@@ -3284,16 +3455,18 @@
       <c r="CG50" s="20"/>
     </row>
     <row r="51" spans="1:85" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="52">
+      <c r="A51" s="58">
         <v>13</v>
       </c>
-      <c r="B51" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="C51" s="49"/>
-      <c r="D51" s="49"/>
-      <c r="E51" s="39" t="s">
-        <v>5</v>
+      <c r="B51" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C51" s="64" t="s">
+        <v>30</v>
+      </c>
+      <c r="D51" s="64"/>
+      <c r="E51" s="26" t="s">
+        <v>25</v>
       </c>
       <c r="F51" s="9"/>
       <c r="M51" s="11"/>
@@ -3316,13 +3489,13 @@
       <c r="BZ51" s="9"/>
       <c r="CG51" s="11"/>
     </row>
-    <row r="52" spans="1:85" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A52" s="52"/>
-      <c r="B52" s="60"/>
-      <c r="C52" s="50"/>
-      <c r="D52" s="50"/>
-      <c r="E52" s="40" t="s">
-        <v>7</v>
+    <row r="52" spans="1:85" s="12" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="58"/>
+      <c r="B52" s="56"/>
+      <c r="C52" s="65"/>
+      <c r="D52" s="65"/>
+      <c r="E52" s="43" t="s">
+        <v>37</v>
       </c>
       <c r="M52" s="13"/>
       <c r="U52" s="13"/>
@@ -3336,12 +3509,12 @@
       <c r="CG52" s="13"/>
     </row>
     <row r="53" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="52"/>
-      <c r="B53" s="60"/>
-      <c r="C53" s="50"/>
-      <c r="D53" s="50"/>
-      <c r="E53" s="41" t="s">
-        <v>9</v>
+      <c r="A53" s="58"/>
+      <c r="B53" s="56"/>
+      <c r="C53" s="65"/>
+      <c r="D53" s="65"/>
+      <c r="E53" s="27" t="s">
+        <v>27</v>
       </c>
       <c r="M53" s="13"/>
       <c r="U53" s="13"/>
@@ -3354,13 +3527,13 @@
       <c r="BY53" s="13"/>
       <c r="CG53" s="13"/>
     </row>
-    <row r="54" spans="1:85" s="14" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A54" s="52"/>
-      <c r="B54" s="61"/>
-      <c r="C54" s="51"/>
-      <c r="D54" s="51"/>
-      <c r="E54" s="40" t="s">
-        <v>10</v>
+    <row r="54" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="58"/>
+      <c r="B54" s="57"/>
+      <c r="C54" s="66"/>
+      <c r="D54" s="66"/>
+      <c r="E54" s="43" t="s">
+        <v>36</v>
       </c>
       <c r="F54" s="12"/>
       <c r="G54" s="12"/>
@@ -3444,16 +3617,21 @@
       <c r="CG54" s="13"/>
     </row>
     <row r="55" spans="1:85" s="16" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="52">
+      <c r="A55" s="58">
         <v>14</v>
       </c>
-      <c r="B55" s="56"/>
-      <c r="C55" s="55"/>
-      <c r="D55" s="56"/>
+      <c r="B55" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="C55" s="69" t="s">
+        <v>35</v>
+      </c>
+      <c r="D55" s="70"/>
       <c r="E55" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="F55" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="F55" s="75"/>
+      <c r="G55" s="73"/>
       <c r="M55" s="17"/>
       <c r="N55" s="15"/>
       <c r="U55" s="17"/>
@@ -3474,15 +3652,15 @@
       <c r="BZ55" s="15"/>
       <c r="CG55" s="17"/>
     </row>
-    <row r="56" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="52"/>
-      <c r="B56" s="53"/>
-      <c r="C56" s="57"/>
-      <c r="D56" s="58"/>
-      <c r="E56" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="F56" s="18"/>
+    <row r="56" spans="1:85" s="19" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="58"/>
+      <c r="B56" s="50"/>
+      <c r="C56" s="71"/>
+      <c r="D56" s="72"/>
+      <c r="E56" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="F56" s="74"/>
       <c r="M56" s="20"/>
       <c r="N56" s="18"/>
       <c r="U56" s="20"/>
@@ -3504,14 +3682,15 @@
       <c r="CG56" s="20"/>
     </row>
     <row r="57" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="52"/>
-      <c r="B57" s="53"/>
-      <c r="C57" s="57"/>
-      <c r="D57" s="58"/>
+      <c r="A57" s="58"/>
+      <c r="B57" s="50"/>
+      <c r="C57" s="71"/>
+      <c r="D57" s="72"/>
       <c r="E57" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F57" s="18"/>
+        <v>27</v>
+      </c>
+      <c r="F57" s="75"/>
+      <c r="G57" s="73"/>
       <c r="M57" s="20"/>
       <c r="N57" s="18"/>
       <c r="U57" s="20"/>
@@ -3532,15 +3711,15 @@
       <c r="BZ57" s="18"/>
       <c r="CG57" s="20"/>
     </row>
-    <row r="58" spans="1:85" s="21" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="52"/>
-      <c r="B58" s="54"/>
-      <c r="C58" s="58"/>
-      <c r="D58" s="58"/>
+    <row r="58" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="58"/>
+      <c r="B58" s="51"/>
+      <c r="C58" s="72"/>
+      <c r="D58" s="72"/>
       <c r="E58" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="F58" s="18"/>
+        <v>36</v>
+      </c>
+      <c r="F58" s="74"/>
       <c r="G58" s="19"/>
       <c r="H58" s="19"/>
       <c r="I58" s="19"/>
@@ -3622,14 +3801,16 @@
       <c r="CG58" s="20"/>
     </row>
     <row r="59" spans="1:85" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="52">
+      <c r="A59" s="58">
         <v>15</v>
       </c>
-      <c r="B59" s="59"/>
-      <c r="C59" s="49"/>
-      <c r="D59" s="49"/>
-      <c r="E59" s="39" t="s">
-        <v>5</v>
+      <c r="B59" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C59" s="64"/>
+      <c r="D59" s="64"/>
+      <c r="E59" s="26" t="s">
+        <v>25</v>
       </c>
       <c r="F59" s="9"/>
       <c r="M59" s="11"/>
@@ -3652,13 +3833,13 @@
       <c r="BZ59" s="9"/>
       <c r="CG59" s="11"/>
     </row>
-    <row r="60" spans="1:85" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A60" s="52"/>
-      <c r="B60" s="60"/>
-      <c r="C60" s="50"/>
-      <c r="D60" s="50"/>
-      <c r="E60" s="40" t="s">
-        <v>7</v>
+    <row r="60" spans="1:85" s="12" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="58"/>
+      <c r="B60" s="47"/>
+      <c r="C60" s="65"/>
+      <c r="D60" s="65"/>
+      <c r="E60" s="43" t="s">
+        <v>37</v>
       </c>
       <c r="M60" s="13"/>
       <c r="U60" s="13"/>
@@ -3672,12 +3853,12 @@
       <c r="CG60" s="13"/>
     </row>
     <row r="61" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="52"/>
-      <c r="B61" s="60"/>
-      <c r="C61" s="50"/>
-      <c r="D61" s="50"/>
-      <c r="E61" s="41" t="s">
-        <v>9</v>
+      <c r="A61" s="58"/>
+      <c r="B61" s="47"/>
+      <c r="C61" s="65"/>
+      <c r="D61" s="65"/>
+      <c r="E61" s="27" t="s">
+        <v>27</v>
       </c>
       <c r="M61" s="13"/>
       <c r="U61" s="13"/>
@@ -3690,13 +3871,13 @@
       <c r="BY61" s="13"/>
       <c r="CG61" s="13"/>
     </row>
-    <row r="62" spans="1:85" s="14" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A62" s="52"/>
-      <c r="B62" s="61"/>
-      <c r="C62" s="51"/>
-      <c r="D62" s="51"/>
-      <c r="E62" s="40" t="s">
-        <v>10</v>
+    <row r="62" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="58"/>
+      <c r="B62" s="48"/>
+      <c r="C62" s="66"/>
+      <c r="D62" s="66"/>
+      <c r="E62" s="43" t="s">
+        <v>36</v>
       </c>
       <c r="F62" s="12"/>
       <c r="G62" s="12"/>
@@ -3779,409 +3960,196 @@
       <c r="CF62" s="12"/>
       <c r="CG62" s="13"/>
     </row>
-    <row r="63" spans="1:85" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="52">
-        <v>16</v>
-      </c>
-      <c r="B63" s="56"/>
-      <c r="C63" s="55"/>
-      <c r="D63" s="56"/>
-      <c r="E63" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="F63" s="15"/>
-      <c r="M63" s="17"/>
-      <c r="N63" s="15"/>
-      <c r="U63" s="17"/>
-      <c r="V63" s="15"/>
-      <c r="AC63" s="17"/>
-      <c r="AD63" s="15"/>
-      <c r="AK63" s="17"/>
-      <c r="AL63" s="15"/>
-      <c r="AS63" s="17"/>
-      <c r="AT63" s="15"/>
-      <c r="BA63" s="17"/>
-      <c r="BB63" s="15"/>
-      <c r="BI63" s="17"/>
-      <c r="BJ63" s="15"/>
-      <c r="BQ63" s="17"/>
-      <c r="BR63" s="15"/>
-      <c r="BY63" s="17"/>
-      <c r="BZ63" s="15"/>
-      <c r="CG63" s="17"/>
-    </row>
-    <row r="64" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="52"/>
+    <row r="63" spans="1:85" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="59"/>
+      <c r="B63" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" s="54"/>
+      <c r="D63" s="54"/>
+      <c r="E63" s="30"/>
+      <c r="F63" s="31"/>
+      <c r="G63" s="32"/>
+      <c r="H63" s="32"/>
+      <c r="I63" s="32"/>
+      <c r="J63" s="32"/>
+      <c r="K63" s="32"/>
+      <c r="L63" s="32"/>
+      <c r="M63" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="N63" s="31"/>
+      <c r="O63" s="32"/>
+      <c r="P63" s="32"/>
+      <c r="Q63" s="32"/>
+      <c r="R63" s="32"/>
+      <c r="S63" s="32"/>
+      <c r="T63" s="32"/>
+      <c r="U63" s="37"/>
+      <c r="V63" s="31"/>
+      <c r="W63" s="32"/>
+      <c r="X63" s="32"/>
+      <c r="Y63" s="32"/>
+      <c r="Z63" s="32"/>
+      <c r="AA63" s="32"/>
+      <c r="AB63" s="32"/>
+      <c r="AC63" s="37"/>
+      <c r="AD63" s="31"/>
+      <c r="AE63" s="32"/>
+      <c r="AF63" s="32"/>
+      <c r="AG63" s="32"/>
+      <c r="AH63" s="32"/>
+      <c r="AI63" s="32"/>
+      <c r="AJ63" s="32"/>
+      <c r="AK63" s="37"/>
+      <c r="AL63" s="31"/>
+      <c r="AM63" s="32"/>
+      <c r="AN63" s="32"/>
+      <c r="AO63" s="32"/>
+      <c r="AP63" s="32"/>
+      <c r="AQ63" s="32"/>
+      <c r="AR63" s="32"/>
+      <c r="AS63" s="37"/>
+      <c r="AT63" s="31"/>
+      <c r="AU63" s="32"/>
+      <c r="AV63" s="32"/>
+      <c r="AW63" s="32"/>
+      <c r="AX63" s="32"/>
+      <c r="AY63" s="32"/>
+      <c r="AZ63" s="32"/>
+      <c r="BA63" s="37"/>
+      <c r="BB63" s="31"/>
+      <c r="BC63" s="32"/>
+      <c r="BD63" s="32"/>
+      <c r="BE63" s="32"/>
+      <c r="BF63" s="32"/>
+      <c r="BG63" s="32"/>
+      <c r="BH63" s="32"/>
+      <c r="BI63" s="37"/>
+      <c r="BJ63" s="31"/>
+      <c r="BK63" s="32"/>
+      <c r="BL63" s="32"/>
+      <c r="BM63" s="32"/>
+      <c r="BN63" s="32"/>
+      <c r="BO63" s="32"/>
+      <c r="BP63" s="32"/>
+      <c r="BQ63" s="37"/>
+      <c r="BR63" s="31"/>
+      <c r="BS63" s="32"/>
+      <c r="BT63" s="32"/>
+      <c r="BU63" s="32"/>
+      <c r="BV63" s="32"/>
+      <c r="BW63" s="32"/>
+      <c r="BX63" s="32"/>
+      <c r="BY63" s="37"/>
+      <c r="BZ63" s="31"/>
+      <c r="CA63" s="32"/>
+      <c r="CB63" s="32"/>
+      <c r="CC63" s="32"/>
+      <c r="CD63" s="32"/>
+      <c r="CE63" s="32"/>
+      <c r="CF63" s="32"/>
+      <c r="CG63" s="37"/>
+    </row>
+    <row r="64" spans="1:85" s="14" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="59"/>
       <c r="B64" s="53"/>
-      <c r="C64" s="57"/>
-      <c r="D64" s="58"/>
-      <c r="E64" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="F64" s="18"/>
-      <c r="M64" s="20"/>
-      <c r="N64" s="18"/>
-      <c r="U64" s="20"/>
-      <c r="V64" s="18"/>
-      <c r="AC64" s="20"/>
-      <c r="AD64" s="18"/>
-      <c r="AK64" s="20"/>
-      <c r="AL64" s="18"/>
-      <c r="AS64" s="20"/>
-      <c r="AT64" s="18"/>
-      <c r="BA64" s="20"/>
-      <c r="BB64" s="18"/>
-      <c r="BI64" s="20"/>
-      <c r="BJ64" s="18"/>
-      <c r="BQ64" s="20"/>
-      <c r="BR64" s="18"/>
-      <c r="BY64" s="20"/>
-      <c r="BZ64" s="18"/>
-      <c r="CG64" s="20"/>
-    </row>
-    <row r="65" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="52"/>
-      <c r="B65" s="53"/>
-      <c r="C65" s="57"/>
-      <c r="D65" s="58"/>
-      <c r="E65" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F65" s="18"/>
-      <c r="M65" s="20"/>
-      <c r="N65" s="18"/>
-      <c r="U65" s="20"/>
-      <c r="V65" s="18"/>
-      <c r="AC65" s="20"/>
-      <c r="AD65" s="18"/>
-      <c r="AK65" s="20"/>
-      <c r="AL65" s="18"/>
-      <c r="AS65" s="20"/>
-      <c r="AT65" s="18"/>
-      <c r="BA65" s="20"/>
-      <c r="BB65" s="18"/>
-      <c r="BI65" s="20"/>
-      <c r="BJ65" s="18"/>
-      <c r="BQ65" s="20"/>
-      <c r="BR65" s="18"/>
-      <c r="BY65" s="20"/>
-      <c r="BZ65" s="18"/>
-      <c r="CG65" s="20"/>
-    </row>
-    <row r="66" spans="1:85" s="21" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="52"/>
-      <c r="B66" s="54"/>
-      <c r="C66" s="58"/>
-      <c r="D66" s="58"/>
-      <c r="E66" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="F66" s="18"/>
-      <c r="G66" s="19"/>
-      <c r="H66" s="19"/>
-      <c r="I66" s="19"/>
-      <c r="J66" s="19"/>
-      <c r="K66" s="19"/>
-      <c r="L66" s="19"/>
-      <c r="M66" s="20"/>
-      <c r="N66" s="18"/>
-      <c r="O66" s="19"/>
-      <c r="P66" s="19"/>
-      <c r="Q66" s="19"/>
-      <c r="R66" s="19"/>
-      <c r="S66" s="19"/>
-      <c r="T66" s="19"/>
-      <c r="U66" s="20"/>
-      <c r="V66" s="18"/>
-      <c r="W66" s="19"/>
-      <c r="X66" s="19"/>
-      <c r="Y66" s="19"/>
-      <c r="Z66" s="19"/>
-      <c r="AA66" s="19"/>
-      <c r="AB66" s="19"/>
-      <c r="AC66" s="20"/>
-      <c r="AD66" s="18"/>
-      <c r="AE66" s="19"/>
-      <c r="AF66" s="19"/>
-      <c r="AG66" s="19"/>
-      <c r="AH66" s="19"/>
-      <c r="AI66" s="19"/>
-      <c r="AJ66" s="19"/>
-      <c r="AK66" s="20"/>
-      <c r="AL66" s="18"/>
-      <c r="AM66" s="19"/>
-      <c r="AN66" s="19"/>
-      <c r="AO66" s="19"/>
-      <c r="AP66" s="19"/>
-      <c r="AQ66" s="19"/>
-      <c r="AR66" s="19"/>
-      <c r="AS66" s="20"/>
-      <c r="AT66" s="18"/>
-      <c r="AU66" s="19"/>
-      <c r="AV66" s="19"/>
-      <c r="AW66" s="19"/>
-      <c r="AX66" s="19"/>
-      <c r="AY66" s="19"/>
-      <c r="AZ66" s="19"/>
-      <c r="BA66" s="20"/>
-      <c r="BB66" s="18"/>
-      <c r="BC66" s="19"/>
-      <c r="BD66" s="19"/>
-      <c r="BE66" s="19"/>
-      <c r="BF66" s="19"/>
-      <c r="BG66" s="19"/>
-      <c r="BH66" s="19"/>
-      <c r="BI66" s="20"/>
-      <c r="BJ66" s="18"/>
-      <c r="BK66" s="19"/>
-      <c r="BL66" s="19"/>
-      <c r="BM66" s="19"/>
-      <c r="BN66" s="19"/>
-      <c r="BO66" s="19"/>
-      <c r="BP66" s="19"/>
-      <c r="BQ66" s="20"/>
-      <c r="BR66" s="18"/>
-      <c r="BS66" s="19"/>
-      <c r="BT66" s="19"/>
-      <c r="BU66" s="19"/>
-      <c r="BV66" s="19"/>
-      <c r="BW66" s="19"/>
-      <c r="BX66" s="19"/>
-      <c r="BY66" s="20"/>
-      <c r="BZ66" s="18"/>
-      <c r="CA66" s="19"/>
-      <c r="CB66" s="19"/>
-      <c r="CC66" s="19"/>
-      <c r="CD66" s="19"/>
-      <c r="CE66" s="19"/>
-      <c r="CF66" s="19"/>
-      <c r="CG66" s="20"/>
-    </row>
-    <row r="67" spans="1:85" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="68"/>
-      <c r="B67" s="69" t="s">
-        <v>4</v>
-      </c>
-      <c r="C67" s="71"/>
-      <c r="D67" s="71"/>
-      <c r="E67" s="30"/>
-      <c r="F67" s="31"/>
-      <c r="G67" s="32"/>
-      <c r="H67" s="32"/>
-      <c r="I67" s="32"/>
-      <c r="J67" s="32"/>
-      <c r="K67" s="32"/>
-      <c r="L67" s="32"/>
-      <c r="M67" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="N67" s="31"/>
-      <c r="O67" s="32"/>
-      <c r="P67" s="32"/>
-      <c r="Q67" s="32"/>
-      <c r="R67" s="32"/>
-      <c r="S67" s="32"/>
-      <c r="T67" s="32"/>
-      <c r="U67" s="37"/>
-      <c r="V67" s="31"/>
-      <c r="W67" s="32"/>
-      <c r="X67" s="32"/>
-      <c r="Y67" s="32"/>
-      <c r="Z67" s="32"/>
-      <c r="AA67" s="32"/>
-      <c r="AB67" s="32"/>
-      <c r="AC67" s="37"/>
-      <c r="AD67" s="31"/>
-      <c r="AE67" s="32"/>
-      <c r="AF67" s="32"/>
-      <c r="AG67" s="32"/>
-      <c r="AH67" s="32"/>
-      <c r="AI67" s="32"/>
-      <c r="AJ67" s="32"/>
-      <c r="AK67" s="37"/>
-      <c r="AL67" s="31"/>
-      <c r="AM67" s="32"/>
-      <c r="AN67" s="32"/>
-      <c r="AO67" s="32"/>
-      <c r="AP67" s="32"/>
-      <c r="AQ67" s="32"/>
-      <c r="AR67" s="32"/>
-      <c r="AS67" s="37"/>
-      <c r="AT67" s="31"/>
-      <c r="AU67" s="32"/>
-      <c r="AV67" s="32"/>
-      <c r="AW67" s="32"/>
-      <c r="AX67" s="32"/>
-      <c r="AY67" s="32"/>
-      <c r="AZ67" s="32"/>
-      <c r="BA67" s="37"/>
-      <c r="BB67" s="31"/>
-      <c r="BC67" s="32"/>
-      <c r="BD67" s="32"/>
-      <c r="BE67" s="32"/>
-      <c r="BF67" s="32"/>
-      <c r="BG67" s="32"/>
-      <c r="BH67" s="32"/>
-      <c r="BI67" s="37"/>
-      <c r="BJ67" s="31"/>
-      <c r="BK67" s="32"/>
-      <c r="BL67" s="32"/>
-      <c r="BM67" s="32"/>
-      <c r="BN67" s="32"/>
-      <c r="BO67" s="32"/>
-      <c r="BP67" s="32"/>
-      <c r="BQ67" s="37"/>
-      <c r="BR67" s="31"/>
-      <c r="BS67" s="32"/>
-      <c r="BT67" s="32"/>
-      <c r="BU67" s="32"/>
-      <c r="BV67" s="32"/>
-      <c r="BW67" s="32"/>
-      <c r="BX67" s="32"/>
-      <c r="BY67" s="37"/>
-      <c r="BZ67" s="31"/>
-      <c r="CA67" s="32"/>
-      <c r="CB67" s="32"/>
-      <c r="CC67" s="32"/>
-      <c r="CD67" s="32"/>
-      <c r="CE67" s="32"/>
-      <c r="CF67" s="32"/>
-      <c r="CG67" s="37"/>
-    </row>
-    <row r="68" spans="1:85" s="14" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="68"/>
-      <c r="B68" s="70"/>
-      <c r="C68" s="72"/>
-      <c r="D68" s="72"/>
-      <c r="E68" s="33"/>
-      <c r="F68" s="34"/>
-      <c r="G68" s="35"/>
-      <c r="H68" s="35"/>
-      <c r="I68" s="35"/>
-      <c r="J68" s="35"/>
-      <c r="K68" s="35"/>
-      <c r="L68" s="35"/>
-      <c r="M68" s="36"/>
-      <c r="N68" s="34"/>
-      <c r="O68" s="35"/>
-      <c r="P68" s="35"/>
-      <c r="Q68" s="35"/>
-      <c r="R68" s="35"/>
-      <c r="S68" s="35"/>
-      <c r="T68" s="35"/>
-      <c r="U68" s="36"/>
-      <c r="V68" s="34"/>
-      <c r="W68" s="35"/>
-      <c r="X68" s="35"/>
-      <c r="Y68" s="35"/>
-      <c r="Z68" s="35"/>
-      <c r="AA68" s="35"/>
-      <c r="AB68" s="35"/>
-      <c r="AC68" s="36"/>
-      <c r="AD68" s="34"/>
-      <c r="AE68" s="35"/>
-      <c r="AF68" s="35"/>
-      <c r="AG68" s="35"/>
-      <c r="AH68" s="35"/>
-      <c r="AI68" s="35"/>
-      <c r="AJ68" s="35"/>
-      <c r="AK68" s="36"/>
-      <c r="AL68" s="34"/>
-      <c r="AM68" s="35"/>
-      <c r="AN68" s="35"/>
-      <c r="AO68" s="35"/>
-      <c r="AP68" s="35"/>
-      <c r="AQ68" s="35"/>
-      <c r="AR68" s="35"/>
-      <c r="AS68" s="36"/>
-      <c r="AT68" s="34"/>
-      <c r="AU68" s="35"/>
-      <c r="AV68" s="35"/>
-      <c r="AW68" s="35"/>
-      <c r="AX68" s="35"/>
-      <c r="AY68" s="35"/>
-      <c r="AZ68" s="35"/>
-      <c r="BA68" s="36"/>
-      <c r="BB68" s="34"/>
-      <c r="BC68" s="35"/>
-      <c r="BD68" s="35"/>
-      <c r="BE68" s="35"/>
-      <c r="BF68" s="35"/>
-      <c r="BG68" s="35"/>
-      <c r="BH68" s="35"/>
-      <c r="BI68" s="36"/>
-      <c r="BJ68" s="34"/>
-      <c r="BK68" s="35"/>
-      <c r="BL68" s="35"/>
-      <c r="BM68" s="35"/>
-      <c r="BN68" s="35"/>
-      <c r="BO68" s="35"/>
-      <c r="BP68" s="35"/>
-      <c r="BQ68" s="36"/>
-      <c r="BR68" s="34"/>
-      <c r="BS68" s="35"/>
-      <c r="BT68" s="35"/>
-      <c r="BU68" s="35"/>
-      <c r="BV68" s="35"/>
-      <c r="BW68" s="35"/>
-      <c r="BX68" s="35"/>
-      <c r="BY68" s="36"/>
-      <c r="BZ68" s="34"/>
-      <c r="CA68" s="35"/>
-      <c r="CB68" s="35"/>
-      <c r="CC68" s="35"/>
-      <c r="CD68" s="35"/>
-      <c r="CE68" s="35"/>
-      <c r="CF68" s="35"/>
-      <c r="CG68" s="36"/>
+      <c r="C64" s="55"/>
+      <c r="D64" s="55"/>
+      <c r="E64" s="33"/>
+      <c r="F64" s="34"/>
+      <c r="G64" s="35"/>
+      <c r="H64" s="35"/>
+      <c r="I64" s="35"/>
+      <c r="J64" s="35"/>
+      <c r="K64" s="35"/>
+      <c r="L64" s="35"/>
+      <c r="M64" s="36"/>
+      <c r="N64" s="34"/>
+      <c r="O64" s="35"/>
+      <c r="P64" s="35"/>
+      <c r="Q64" s="35"/>
+      <c r="R64" s="35"/>
+      <c r="S64" s="35"/>
+      <c r="T64" s="35"/>
+      <c r="U64" s="36"/>
+      <c r="V64" s="34"/>
+      <c r="W64" s="35"/>
+      <c r="X64" s="35"/>
+      <c r="Y64" s="35"/>
+      <c r="Z64" s="35"/>
+      <c r="AA64" s="35"/>
+      <c r="AB64" s="35"/>
+      <c r="AC64" s="36"/>
+      <c r="AD64" s="34"/>
+      <c r="AE64" s="35"/>
+      <c r="AF64" s="35"/>
+      <c r="AG64" s="35"/>
+      <c r="AH64" s="35"/>
+      <c r="AI64" s="35"/>
+      <c r="AJ64" s="35"/>
+      <c r="AK64" s="36"/>
+      <c r="AL64" s="34"/>
+      <c r="AM64" s="35"/>
+      <c r="AN64" s="35"/>
+      <c r="AO64" s="35"/>
+      <c r="AP64" s="35"/>
+      <c r="AQ64" s="35"/>
+      <c r="AR64" s="35"/>
+      <c r="AS64" s="36"/>
+      <c r="AT64" s="34"/>
+      <c r="AU64" s="35"/>
+      <c r="AV64" s="35"/>
+      <c r="AW64" s="35"/>
+      <c r="AX64" s="35"/>
+      <c r="AY64" s="35"/>
+      <c r="AZ64" s="35"/>
+      <c r="BA64" s="36"/>
+      <c r="BB64" s="34"/>
+      <c r="BC64" s="35"/>
+      <c r="BD64" s="35"/>
+      <c r="BE64" s="35"/>
+      <c r="BF64" s="35"/>
+      <c r="BG64" s="35"/>
+      <c r="BH64" s="35"/>
+      <c r="BI64" s="36"/>
+      <c r="BJ64" s="34"/>
+      <c r="BK64" s="35"/>
+      <c r="BL64" s="35"/>
+      <c r="BM64" s="35"/>
+      <c r="BN64" s="35"/>
+      <c r="BO64" s="35"/>
+      <c r="BP64" s="35"/>
+      <c r="BQ64" s="36"/>
+      <c r="BR64" s="34"/>
+      <c r="BS64" s="35"/>
+      <c r="BT64" s="35"/>
+      <c r="BU64" s="35"/>
+      <c r="BV64" s="35"/>
+      <c r="BW64" s="35"/>
+      <c r="BX64" s="35"/>
+      <c r="BY64" s="36"/>
+      <c r="BZ64" s="34"/>
+      <c r="CA64" s="35"/>
+      <c r="CB64" s="35"/>
+      <c r="CC64" s="35"/>
+      <c r="CD64" s="35"/>
+      <c r="CE64" s="35"/>
+      <c r="CF64" s="35"/>
+      <c r="CG64" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="63">
-    <mergeCell ref="C51:D54"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:D68"/>
-    <mergeCell ref="C55:D58"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="C59:D62"/>
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="C63:D66"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="A63:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="B51:B54"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="BB1:BI1"/>
-    <mergeCell ref="C7:D10"/>
-    <mergeCell ref="F1:M1"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:D6"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:D14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="C15:D18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:D22"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:D26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:D30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="C31:D34"/>
+  <mergeCells count="61">
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="BJ1:BQ1"/>
+    <mergeCell ref="BR1:BY1"/>
+    <mergeCell ref="BZ1:CG1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="V1:AC1"/>
+    <mergeCell ref="AD1:AK1"/>
+    <mergeCell ref="AL1:AS1"/>
+    <mergeCell ref="AT1:BA1"/>
     <mergeCell ref="C43:D46"/>
     <mergeCell ref="A47:A50"/>
     <mergeCell ref="B47:B50"/>
@@ -4192,14 +4160,47 @@
     <mergeCell ref="A39:A42"/>
     <mergeCell ref="B39:B42"/>
     <mergeCell ref="C39:D42"/>
-    <mergeCell ref="BJ1:BQ1"/>
-    <mergeCell ref="BR1:BY1"/>
-    <mergeCell ref="BZ1:CG1"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="V1:AC1"/>
-    <mergeCell ref="AD1:AK1"/>
-    <mergeCell ref="AL1:AS1"/>
-    <mergeCell ref="AT1:BA1"/>
+    <mergeCell ref="C23:D26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:D30"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="C31:D34"/>
+    <mergeCell ref="C11:D14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C15:D18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:D22"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="BB1:BI1"/>
+    <mergeCell ref="C7:D10"/>
+    <mergeCell ref="F1:M1"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:D6"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C51:D54"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="C63:D64"/>
+    <mergeCell ref="C55:D58"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="C59:D62"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>